<commit_message>
mysql init database finished
</commit_message>
<xml_diff>
--- a/xls/schema/data/laundry.xlsx
+++ b/xls/schema/data/laundry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13840" yWindow="2840" windowWidth="25600" windowHeight="16060" tabRatio="432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="432" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TB_WORK_STATION" sheetId="2" r:id="rId1"/>
@@ -870,7 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -1363,7 +1363,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1829,7 +1828,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1842,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2104,7 +2102,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>